<commit_message>
V2 of the program
now with an excel with velocities and mileage
</commit_message>
<xml_diff>
--- a/CH4_reducido.xlsx
+++ b/CH4_reducido.xlsx
@@ -699,7 +699,7 @@
         <v>0.131</v>
       </c>
       <c r="Z2">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA2">
         <v>100</v>
@@ -770,7 +770,7 @@
         <v>0.041</v>
       </c>
       <c r="Z3">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA3">
         <v>100</v>
@@ -841,7 +841,7 @@
         <v>0.026</v>
       </c>
       <c r="Z4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA4">
         <v>100</v>
@@ -912,7 +912,7 @@
         <v>0.014</v>
       </c>
       <c r="Z5">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA5">
         <v>100</v>
@@ -983,7 +983,7 @@
         <v>0.017</v>
       </c>
       <c r="Z6">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA6">
         <v>100</v>
@@ -1054,7 +1054,7 @@
         <v>0.011</v>
       </c>
       <c r="Z7">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA7">
         <v>100</v>
@@ -1128,7 +1128,7 @@
         <v>0.003</v>
       </c>
       <c r="Z8">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA8">
         <v>100</v>
@@ -1202,7 +1202,7 @@
         <v>0.004</v>
       </c>
       <c r="Z9">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA9">
         <v>100</v>
@@ -1276,7 +1276,7 @@
         <v>0.00287</v>
       </c>
       <c r="Z10">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA10">
         <v>100</v>
@@ -1350,7 +1350,7 @@
         <v>0.00508</v>
       </c>
       <c r="Z11">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA11">
         <v>100</v>
@@ -1424,7 +1424,7 @@
         <v>0.00287</v>
       </c>
       <c r="Z12">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA12">
         <v>100</v>
@@ -1498,7 +1498,7 @@
         <v>0.00508</v>
       </c>
       <c r="Z13">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA13">
         <v>100</v>
@@ -1572,7 +1572,7 @@
         <v>0.00287</v>
       </c>
       <c r="Z14">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA14">
         <v>100</v>
@@ -1646,7 +1646,7 @@
         <v>0.00508</v>
       </c>
       <c r="Z15">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA15">
         <v>100</v>
@@ -1720,7 +1720,7 @@
         <v>0.00287</v>
       </c>
       <c r="Z16">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA16">
         <v>100</v>
@@ -1794,7 +1794,7 @@
         <v>0.00508</v>
       </c>
       <c r="Z17">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA17">
         <v>100</v>
@@ -1865,7 +1865,7 @@
         <v>0.028</v>
       </c>
       <c r="Z18">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA18">
         <v>100</v>
@@ -1936,7 +1936,7 @@
         <v>0.008</v>
       </c>
       <c r="Z19">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA19">
         <v>100</v>
@@ -2007,7 +2007,7 @@
         <v>0.011</v>
       </c>
       <c r="Z20">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA20">
         <v>100</v>
@@ -2078,7 +2078,7 @@
         <v>0.003</v>
       </c>
       <c r="Z21">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA21">
         <v>100</v>
@@ -2149,7 +2149,7 @@
         <v>0.007</v>
       </c>
       <c r="Z22">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA22">
         <v>100</v>
@@ -2220,7 +2220,7 @@
         <v>0.002</v>
       </c>
       <c r="Z23">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA23">
         <v>100</v>
@@ -2294,7 +2294,7 @@
         <v>0.003</v>
       </c>
       <c r="Z24">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA24">
         <v>100</v>
@@ -2368,7 +2368,7 @@
         <v>0</v>
       </c>
       <c r="Z25">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA25">
         <v>100</v>
@@ -2442,7 +2442,7 @@
         <v>0.0011</v>
       </c>
       <c r="Z26">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA26">
         <v>100</v>
@@ -2516,7 +2516,7 @@
         <v>0</v>
       </c>
       <c r="Z27">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA27">
         <v>100</v>
@@ -2590,7 +2590,7 @@
         <v>7.499999999999999E-05</v>
       </c>
       <c r="Z28">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA28">
         <v>100</v>
@@ -2664,7 +2664,7 @@
         <v>0</v>
       </c>
       <c r="Z29">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA29">
         <v>100</v>
@@ -2738,7 +2738,7 @@
         <v>7.499999999999999E-05</v>
       </c>
       <c r="Z30">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA30">
         <v>100</v>
@@ -2812,7 +2812,7 @@
         <v>0</v>
       </c>
       <c r="Z31">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA31">
         <v>100</v>
@@ -2886,7 +2886,7 @@
         <v>7.499999999999999E-05</v>
       </c>
       <c r="Z32">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA32">
         <v>100</v>
@@ -2960,7 +2960,7 @@
         <v>0</v>
       </c>
       <c r="Z33">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA33">
         <v>100</v>
@@ -3034,7 +3034,7 @@
         <v>7.499999999999999E-05</v>
       </c>
       <c r="Z34">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA34">
         <v>100</v>
@@ -3108,7 +3108,7 @@
         <v>0</v>
       </c>
       <c r="Z35">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA35">
         <v>100</v>
@@ -3182,7 +3182,7 @@
         <v>7.499999999999999E-05</v>
       </c>
       <c r="Z36">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA36">
         <v>100</v>
@@ -3256,7 +3256,7 @@
         <v>0</v>
       </c>
       <c r="Z37">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA37">
         <v>100</v>
@@ -3327,7 +3327,7 @@
         <v>0.131</v>
       </c>
       <c r="Z38">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA38">
         <v>100</v>
@@ -3398,7 +3398,7 @@
         <v>0.041</v>
       </c>
       <c r="Z39">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA39">
         <v>100</v>
@@ -3469,7 +3469,7 @@
         <v>0.026</v>
       </c>
       <c r="Z40">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA40">
         <v>100</v>
@@ -3540,7 +3540,7 @@
         <v>0.014</v>
       </c>
       <c r="Z41">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA41">
         <v>100</v>
@@ -3611,7 +3611,7 @@
         <v>0.017</v>
       </c>
       <c r="Z42">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA42">
         <v>100</v>
@@ -3682,7 +3682,7 @@
         <v>0.011</v>
       </c>
       <c r="Z43">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA43">
         <v>100</v>
@@ -3756,7 +3756,7 @@
         <v>0.003</v>
       </c>
       <c r="Z44">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA44">
         <v>100</v>
@@ -3830,7 +3830,7 @@
         <v>0.004</v>
       </c>
       <c r="Z45">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA45">
         <v>100</v>
@@ -3904,7 +3904,7 @@
         <v>0.002</v>
       </c>
       <c r="Z46">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA46">
         <v>100</v>
@@ -3978,7 +3978,7 @@
         <v>0</v>
       </c>
       <c r="Z47">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA47">
         <v>100</v>
@@ -4052,7 +4052,7 @@
         <v>0.002</v>
       </c>
       <c r="Z48">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA48">
         <v>100</v>
@@ -4126,7 +4126,7 @@
         <v>0</v>
       </c>
       <c r="Z49">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA49">
         <v>100</v>
@@ -4200,7 +4200,7 @@
         <v>0.002</v>
       </c>
       <c r="Z50">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA50">
         <v>100</v>
@@ -4274,7 +4274,7 @@
         <v>0</v>
       </c>
       <c r="Z51">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA51">
         <v>100</v>
@@ -4348,7 +4348,7 @@
         <v>0.002</v>
       </c>
       <c r="Z52">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA52">
         <v>100</v>
@@ -4422,7 +4422,7 @@
         <v>0</v>
       </c>
       <c r="Z53">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA53">
         <v>100</v>
@@ -4493,7 +4493,7 @@
         <v>0.028</v>
       </c>
       <c r="Z54">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA54">
         <v>100</v>
@@ -4564,7 +4564,7 @@
         <v>0.008</v>
       </c>
       <c r="Z55">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA55">
         <v>100</v>
@@ -4635,7 +4635,7 @@
         <v>0.011</v>
       </c>
       <c r="Z56">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA56">
         <v>100</v>
@@ -4706,7 +4706,7 @@
         <v>0.003</v>
       </c>
       <c r="Z57">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA57">
         <v>100</v>
@@ -4777,7 +4777,7 @@
         <v>0.007</v>
       </c>
       <c r="Z58">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA58">
         <v>100</v>
@@ -4848,7 +4848,7 @@
         <v>0.002</v>
       </c>
       <c r="Z59">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA59">
         <v>100</v>
@@ -4922,7 +4922,7 @@
         <v>0.003</v>
       </c>
       <c r="Z60">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA60">
         <v>100</v>
@@ -4996,7 +4996,7 @@
         <v>0</v>
       </c>
       <c r="Z61">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA61">
         <v>100</v>
@@ -5070,7 +5070,7 @@
         <v>0.0011</v>
       </c>
       <c r="Z62">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA62">
         <v>100</v>
@@ -5144,7 +5144,7 @@
         <v>0</v>
       </c>
       <c r="Z63">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA63">
         <v>100</v>
@@ -5218,7 +5218,7 @@
         <v>7.499999999999999E-06</v>
       </c>
       <c r="Z64">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA64">
         <v>100</v>
@@ -5292,7 +5292,7 @@
         <v>0</v>
       </c>
       <c r="Z65">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA65">
         <v>100</v>
@@ -5366,7 +5366,7 @@
         <v>7.499999999999999E-06</v>
       </c>
       <c r="Z66">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA66">
         <v>100</v>
@@ -5440,7 +5440,7 @@
         <v>0</v>
       </c>
       <c r="Z67">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA67">
         <v>100</v>
@@ -5514,7 +5514,7 @@
         <v>7.499999999999999E-06</v>
       </c>
       <c r="Z68">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA68">
         <v>100</v>
@@ -5588,7 +5588,7 @@
         <v>0</v>
       </c>
       <c r="Z69">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA69">
         <v>100</v>
@@ -5662,7 +5662,7 @@
         <v>7.499999999999999E-06</v>
       </c>
       <c r="Z70">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA70">
         <v>100</v>
@@ -5736,7 +5736,7 @@
         <v>0</v>
       </c>
       <c r="Z71">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA71">
         <v>100</v>
@@ -5810,7 +5810,7 @@
         <v>7.499999999999999E-06</v>
       </c>
       <c r="Z72">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA72">
         <v>100</v>
@@ -5884,7 +5884,7 @@
         <v>0</v>
       </c>
       <c r="Z73">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA73">
         <v>100</v>
@@ -5955,7 +5955,7 @@
         <v>0.08500000000000001</v>
       </c>
       <c r="Z74">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA74">
         <v>90</v>
@@ -6026,7 +6026,7 @@
         <v>0.02</v>
       </c>
       <c r="Z75">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA75">
         <v>90</v>
@@ -6097,7 +6097,7 @@
         <v>0.08500000000000001</v>
       </c>
       <c r="Z76">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA76">
         <v>90</v>
@@ -6168,7 +6168,7 @@
         <v>0.02</v>
       </c>
       <c r="Z77">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA77">
         <v>90</v>
@@ -6239,7 +6239,7 @@
         <v>0.0544</v>
       </c>
       <c r="Z78">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA78">
         <v>90</v>
@@ -6310,7 +6310,7 @@
         <v>0.0186</v>
       </c>
       <c r="Z79">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA79">
         <v>90</v>
@@ -6381,7 +6381,7 @@
         <v>0.04760000000000001</v>
       </c>
       <c r="Z80">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA80">
         <v>90</v>
@@ -6452,7 +6452,7 @@
         <v>0.0182</v>
       </c>
       <c r="Z81">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA81">
         <v>90</v>
@@ -6526,7 +6526,7 @@
         <v>0.002550000000000002</v>
       </c>
       <c r="Z82">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA82">
         <v>90</v>
@@ -6600,7 +6600,7 @@
         <v>0.001200000000000001</v>
       </c>
       <c r="Z83">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA83">
         <v>90</v>
@@ -6674,7 +6674,7 @@
         <v>0.002550000000000002</v>
       </c>
       <c r="Z84">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA84">
         <v>90</v>
@@ -6748,7 +6748,7 @@
         <v>0.001200000000000001</v>
       </c>
       <c r="Z85">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA85">
         <v>90</v>
@@ -6822,7 +6822,7 @@
         <v>0.002550000000000002</v>
       </c>
       <c r="Z86">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA86">
         <v>90</v>
@@ -6896,7 +6896,7 @@
         <v>0.001200000000000001</v>
       </c>
       <c r="Z87">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA87">
         <v>90</v>
@@ -6970,7 +6970,7 @@
         <v>0.002550000000000002</v>
       </c>
       <c r="Z88">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA88">
         <v>90</v>
@@ -7044,7 +7044,7 @@
         <v>0.001200000000000001</v>
       </c>
       <c r="Z89">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA89">
         <v>90</v>
@@ -7115,7 +7115,7 @@
         <v>0.08500000000000001</v>
       </c>
       <c r="Z90">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA90">
         <v>90</v>
@@ -7186,7 +7186,7 @@
         <v>0.02</v>
       </c>
       <c r="Z91">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA91">
         <v>90</v>
@@ -7257,7 +7257,7 @@
         <v>0.08500000000000001</v>
       </c>
       <c r="Z92">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA92">
         <v>90</v>
@@ -7328,7 +7328,7 @@
         <v>0.02</v>
       </c>
       <c r="Z93">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA93">
         <v>90</v>
@@ -7399,7 +7399,7 @@
         <v>0.0544</v>
       </c>
       <c r="Z94">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA94">
         <v>90</v>
@@ -7470,7 +7470,7 @@
         <v>0.0186</v>
       </c>
       <c r="Z95">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA95">
         <v>90</v>
@@ -7541,7 +7541,7 @@
         <v>0.04760000000000001</v>
       </c>
       <c r="Z96">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA96">
         <v>90</v>
@@ -7612,7 +7612,7 @@
         <v>0.0182</v>
       </c>
       <c r="Z97">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA97">
         <v>90</v>
@@ -7686,7 +7686,7 @@
         <v>0.002550000000000002</v>
       </c>
       <c r="Z98">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA98">
         <v>90</v>
@@ -7760,7 +7760,7 @@
         <v>0.001200000000000001</v>
       </c>
       <c r="Z99">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA99">
         <v>90</v>
@@ -7834,7 +7834,7 @@
         <v>0.002550000000000002</v>
       </c>
       <c r="Z100">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA100">
         <v>90</v>
@@ -7908,7 +7908,7 @@
         <v>0.001200000000000001</v>
       </c>
       <c r="Z101">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA101">
         <v>90</v>
@@ -7982,7 +7982,7 @@
         <v>0.002550000000000002</v>
       </c>
       <c r="Z102">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA102">
         <v>90</v>
@@ -8056,7 +8056,7 @@
         <v>0.001200000000000001</v>
       </c>
       <c r="Z103">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA103">
         <v>90</v>
@@ -8130,7 +8130,7 @@
         <v>0.002550000000000002</v>
       </c>
       <c r="Z104">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA104">
         <v>90</v>
@@ -8204,7 +8204,7 @@
         <v>0.001200000000000001</v>
       </c>
       <c r="Z105">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA105">
         <v>90</v>
@@ -8275,7 +8275,7 @@
         <v>0.08500000000000001</v>
       </c>
       <c r="Z106">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA106">
         <v>90</v>
@@ -8346,7 +8346,7 @@
         <v>0.02</v>
       </c>
       <c r="Z107">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA107">
         <v>90</v>
@@ -8417,7 +8417,7 @@
         <v>0.08500000000000001</v>
       </c>
       <c r="Z108">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA108">
         <v>90</v>
@@ -8488,7 +8488,7 @@
         <v>0.02</v>
       </c>
       <c r="Z109">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA109">
         <v>90</v>
@@ -8559,7 +8559,7 @@
         <v>0.0544</v>
       </c>
       <c r="Z110">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA110">
         <v>90</v>
@@ -8630,7 +8630,7 @@
         <v>0.0186</v>
       </c>
       <c r="Z111">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA111">
         <v>90</v>
@@ -8701,7 +8701,7 @@
         <v>0.04760000000000001</v>
       </c>
       <c r="Z112">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA112">
         <v>90</v>
@@ -8772,7 +8772,7 @@
         <v>0.0182</v>
       </c>
       <c r="Z113">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA113">
         <v>90</v>
@@ -8846,7 +8846,7 @@
         <v>0.002550000000000002</v>
       </c>
       <c r="Z114">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA114">
         <v>90</v>
@@ -8920,7 +8920,7 @@
         <v>0.001200000000000001</v>
       </c>
       <c r="Z115">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA115">
         <v>90</v>
@@ -8994,7 +8994,7 @@
         <v>0.002550000000000002</v>
       </c>
       <c r="Z116">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA116">
         <v>90</v>
@@ -9068,7 +9068,7 @@
         <v>0.001200000000000001</v>
       </c>
       <c r="Z117">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA117">
         <v>90</v>
@@ -9142,7 +9142,7 @@
         <v>0.002550000000000002</v>
       </c>
       <c r="Z118">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA118">
         <v>90</v>
@@ -9216,7 +9216,7 @@
         <v>0.001200000000000001</v>
       </c>
       <c r="Z119">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA119">
         <v>90</v>
@@ -9290,7 +9290,7 @@
         <v>0.002550000000000002</v>
       </c>
       <c r="Z120">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA120">
         <v>90</v>
@@ -9364,7 +9364,7 @@
         <v>0.001200000000000001</v>
       </c>
       <c r="Z121">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA121">
         <v>90</v>
@@ -9435,7 +9435,7 @@
         <v>0.175</v>
       </c>
       <c r="Z122">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA122">
         <v>90</v>
@@ -9506,7 +9506,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z123">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA123">
         <v>90</v>
@@ -9577,7 +9577,7 @@
         <v>0.175</v>
       </c>
       <c r="Z124">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA124">
         <v>90</v>
@@ -9648,7 +9648,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z125">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA125">
         <v>90</v>
@@ -9719,7 +9719,7 @@
         <v>0.112</v>
       </c>
       <c r="Z126">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA126">
         <v>90</v>
@@ -9790,7 +9790,7 @@
         <v>0.06510000000000001</v>
       </c>
       <c r="Z127">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA127">
         <v>90</v>
@@ -9861,7 +9861,7 @@
         <v>0.098</v>
       </c>
       <c r="Z128">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA128">
         <v>90</v>
@@ -9932,7 +9932,7 @@
         <v>0.06370000000000001</v>
       </c>
       <c r="Z129">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA129">
         <v>90</v>
@@ -10006,7 +10006,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z130">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA130">
         <v>90</v>
@@ -10080,7 +10080,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z131">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA131">
         <v>90</v>
@@ -10154,7 +10154,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z132">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA132">
         <v>90</v>
@@ -10228,7 +10228,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z133">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA133">
         <v>90</v>
@@ -10302,7 +10302,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z134">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA134">
         <v>90</v>
@@ -10376,7 +10376,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z135">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA135">
         <v>90</v>
@@ -10450,7 +10450,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z136">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA136">
         <v>90</v>
@@ -10524,7 +10524,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z137">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA137">
         <v>90</v>
@@ -10595,7 +10595,7 @@
         <v>0.175</v>
       </c>
       <c r="Z138">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA138">
         <v>90</v>
@@ -10666,7 +10666,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z139">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA139">
         <v>90</v>
@@ -10737,7 +10737,7 @@
         <v>0.175</v>
       </c>
       <c r="Z140">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA140">
         <v>90</v>
@@ -10808,7 +10808,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z141">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA141">
         <v>90</v>
@@ -10879,7 +10879,7 @@
         <v>0.112</v>
       </c>
       <c r="Z142">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA142">
         <v>90</v>
@@ -10950,7 +10950,7 @@
         <v>0.06510000000000001</v>
       </c>
       <c r="Z143">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA143">
         <v>90</v>
@@ -11021,7 +11021,7 @@
         <v>0.098</v>
       </c>
       <c r="Z144">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA144">
         <v>90</v>
@@ -11092,7 +11092,7 @@
         <v>0.06370000000000001</v>
       </c>
       <c r="Z145">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA145">
         <v>90</v>
@@ -11166,7 +11166,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z146">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA146">
         <v>90</v>
@@ -11240,7 +11240,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z147">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA147">
         <v>90</v>
@@ -11314,7 +11314,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z148">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA148">
         <v>90</v>
@@ -11388,7 +11388,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z149">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA149">
         <v>90</v>
@@ -11462,7 +11462,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z150">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA150">
         <v>90</v>
@@ -11536,7 +11536,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z151">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA151">
         <v>90</v>
@@ -11610,7 +11610,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z152">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA152">
         <v>90</v>
@@ -11684,7 +11684,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z153">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA153">
         <v>90</v>
@@ -11755,7 +11755,7 @@
         <v>0.175</v>
       </c>
       <c r="Z154">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA154">
         <v>90</v>
@@ -11826,7 +11826,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z155">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA155">
         <v>90</v>
@@ -11897,7 +11897,7 @@
         <v>0.175</v>
       </c>
       <c r="Z156">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA156">
         <v>90</v>
@@ -11968,7 +11968,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z157">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA157">
         <v>90</v>
@@ -12039,7 +12039,7 @@
         <v>0.112</v>
       </c>
       <c r="Z158">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA158">
         <v>90</v>
@@ -12110,7 +12110,7 @@
         <v>0.06510000000000001</v>
       </c>
       <c r="Z159">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA159">
         <v>90</v>
@@ -12181,7 +12181,7 @@
         <v>0.098</v>
       </c>
       <c r="Z160">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA160">
         <v>90</v>
@@ -12252,7 +12252,7 @@
         <v>0.06370000000000001</v>
       </c>
       <c r="Z161">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA161">
         <v>90</v>
@@ -12326,7 +12326,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z162">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA162">
         <v>90</v>
@@ -12400,7 +12400,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z163">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA163">
         <v>90</v>
@@ -12474,7 +12474,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z164">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA164">
         <v>90</v>
@@ -12548,7 +12548,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z165">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA165">
         <v>90</v>
@@ -12622,7 +12622,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z166">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA166">
         <v>90</v>
@@ -12696,7 +12696,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z167">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA167">
         <v>90</v>
@@ -12770,7 +12770,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z168">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA168">
         <v>90</v>
@@ -12844,7 +12844,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z169">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA169">
         <v>90</v>
@@ -12915,7 +12915,7 @@
         <v>0.175</v>
       </c>
       <c r="Z170">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA170">
         <v>80</v>
@@ -12986,7 +12986,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z171">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA171">
         <v>80</v>
@@ -13057,7 +13057,7 @@
         <v>0.175</v>
       </c>
       <c r="Z172">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA172">
         <v>80</v>
@@ -13128,7 +13128,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z173">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA173">
         <v>80</v>
@@ -13199,7 +13199,7 @@
         <v>0.112</v>
       </c>
       <c r="Z174">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA174">
         <v>80</v>
@@ -13270,7 +13270,7 @@
         <v>0.06510000000000001</v>
       </c>
       <c r="Z175">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA175">
         <v>80</v>
@@ -13341,7 +13341,7 @@
         <v>0.098</v>
       </c>
       <c r="Z176">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA176">
         <v>80</v>
@@ -13412,7 +13412,7 @@
         <v>0.06370000000000001</v>
       </c>
       <c r="Z177">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA177">
         <v>80</v>
@@ -13486,7 +13486,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z178">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA178">
         <v>80</v>
@@ -13560,7 +13560,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z179">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA179">
         <v>80</v>
@@ -13634,7 +13634,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z180">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA180">
         <v>80</v>
@@ -13708,7 +13708,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z181">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA181">
         <v>80</v>
@@ -13782,7 +13782,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z182">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA182">
         <v>80</v>
@@ -13856,7 +13856,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z183">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA183">
         <v>80</v>
@@ -13930,7 +13930,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z184">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA184">
         <v>80</v>
@@ -14004,7 +14004,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z185">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA185">
         <v>80</v>
@@ -14075,7 +14075,7 @@
         <v>0.175</v>
       </c>
       <c r="Z186">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA186">
         <v>80</v>
@@ -14146,7 +14146,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z187">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA187">
         <v>80</v>
@@ -14217,7 +14217,7 @@
         <v>0.175</v>
       </c>
       <c r="Z188">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA188">
         <v>80</v>
@@ -14288,7 +14288,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z189">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA189">
         <v>80</v>
@@ -14359,7 +14359,7 @@
         <v>0.112</v>
       </c>
       <c r="Z190">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA190">
         <v>80</v>
@@ -14430,7 +14430,7 @@
         <v>0.06510000000000001</v>
       </c>
       <c r="Z191">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA191">
         <v>80</v>
@@ -14501,7 +14501,7 @@
         <v>0.098</v>
       </c>
       <c r="Z192">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA192">
         <v>80</v>
@@ -14572,7 +14572,7 @@
         <v>0.06370000000000001</v>
       </c>
       <c r="Z193">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA193">
         <v>80</v>
@@ -14646,7 +14646,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z194">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA194">
         <v>80</v>
@@ -14720,7 +14720,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z195">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA195">
         <v>80</v>
@@ -14794,7 +14794,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z196">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA196">
         <v>80</v>
@@ -14868,7 +14868,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z197">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA197">
         <v>80</v>
@@ -14942,7 +14942,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z198">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA198">
         <v>80</v>
@@ -15016,7 +15016,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z199">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA199">
         <v>80</v>
@@ -15090,7 +15090,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z200">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA200">
         <v>80</v>
@@ -15164,7 +15164,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z201">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA201">
         <v>80</v>
@@ -15235,7 +15235,7 @@
         <v>0.175</v>
       </c>
       <c r="Z202">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA202">
         <v>80</v>
@@ -15306,7 +15306,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z203">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA203">
         <v>80</v>
@@ -15377,7 +15377,7 @@
         <v>0.175</v>
       </c>
       <c r="Z204">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA204">
         <v>80</v>
@@ -15448,7 +15448,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z205">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA205">
         <v>80</v>
@@ -15519,7 +15519,7 @@
         <v>0.112</v>
       </c>
       <c r="Z206">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA206">
         <v>80</v>
@@ -15590,7 +15590,7 @@
         <v>0.06510000000000001</v>
       </c>
       <c r="Z207">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA207">
         <v>80</v>
@@ -15661,7 +15661,7 @@
         <v>0.098</v>
       </c>
       <c r="Z208">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA208">
         <v>80</v>
@@ -15732,7 +15732,7 @@
         <v>0.06370000000000001</v>
       </c>
       <c r="Z209">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA209">
         <v>80</v>
@@ -15806,7 +15806,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z210">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA210">
         <v>80</v>
@@ -15880,7 +15880,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z211">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA211">
         <v>80</v>
@@ -15954,7 +15954,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z212">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA212">
         <v>80</v>
@@ -16028,7 +16028,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z213">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA213">
         <v>80</v>
@@ -16102,7 +16102,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z214">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA214">
         <v>80</v>
@@ -16176,7 +16176,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z215">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA215">
         <v>80</v>
@@ -16250,7 +16250,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z216">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA216">
         <v>80</v>
@@ -16324,7 +16324,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z217">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA217">
         <v>80</v>
@@ -16395,7 +16395,7 @@
         <v>0.175</v>
       </c>
       <c r="Z218">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA218">
         <v>80</v>
@@ -16466,7 +16466,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z219">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA219">
         <v>80</v>
@@ -16537,7 +16537,7 @@
         <v>0.175</v>
       </c>
       <c r="Z220">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA220">
         <v>80</v>
@@ -16608,7 +16608,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z221">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA221">
         <v>80</v>
@@ -16679,7 +16679,7 @@
         <v>0.112</v>
       </c>
       <c r="Z222">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA222">
         <v>80</v>
@@ -16750,7 +16750,7 @@
         <v>0.06510000000000001</v>
       </c>
       <c r="Z223">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA223">
         <v>80</v>
@@ -16821,7 +16821,7 @@
         <v>0.098</v>
       </c>
       <c r="Z224">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA224">
         <v>80</v>
@@ -16892,7 +16892,7 @@
         <v>0.006999999999999999</v>
       </c>
       <c r="Z225">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA225">
         <v>80</v>
@@ -16966,7 +16966,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z226">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA226">
         <v>80</v>
@@ -17040,7 +17040,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z227">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA227">
         <v>80</v>
@@ -17114,7 +17114,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z228">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA228">
         <v>80</v>
@@ -17188,7 +17188,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z229">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA229">
         <v>80</v>
@@ -17262,7 +17262,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z230">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA230">
         <v>80</v>
@@ -17336,7 +17336,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z231">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA231">
         <v>80</v>
@@ -17410,7 +17410,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z232">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA232">
         <v>80</v>
@@ -17484,7 +17484,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z233">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA233">
         <v>80</v>
@@ -17555,7 +17555,7 @@
         <v>0.175</v>
       </c>
       <c r="Z234">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA234">
         <v>80</v>
@@ -17626,7 +17626,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z235">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA235">
         <v>80</v>
@@ -17697,7 +17697,7 @@
         <v>0.175</v>
       </c>
       <c r="Z236">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA236">
         <v>80</v>
@@ -17768,7 +17768,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z237">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA237">
         <v>80</v>
@@ -17839,7 +17839,7 @@
         <v>0.112</v>
       </c>
       <c r="Z238">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA238">
         <v>80</v>
@@ -17910,7 +17910,7 @@
         <v>0.06510000000000001</v>
       </c>
       <c r="Z239">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA239">
         <v>80</v>
@@ -17981,7 +17981,7 @@
         <v>0.098</v>
       </c>
       <c r="Z240">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA240">
         <v>80</v>
@@ -18052,7 +18052,7 @@
         <v>0.06370000000000001</v>
       </c>
       <c r="Z241">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA241">
         <v>80</v>
@@ -18126,7 +18126,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z242">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA242">
         <v>80</v>
@@ -18200,7 +18200,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z243">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA243">
         <v>80</v>
@@ -18274,7 +18274,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z244">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA244">
         <v>80</v>
@@ -18348,7 +18348,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z245">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA245">
         <v>80</v>
@@ -18422,7 +18422,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z246">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA246">
         <v>80</v>
@@ -18496,7 +18496,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z247">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA247">
         <v>80</v>
@@ -18570,7 +18570,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z248">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA248">
         <v>80</v>
@@ -18644,7 +18644,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z249">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA249">
         <v>80</v>
@@ -18715,7 +18715,7 @@
         <v>0.175</v>
       </c>
       <c r="Z250">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA250">
         <v>80</v>
@@ -18786,7 +18786,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z251">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA251">
         <v>80</v>
@@ -18857,7 +18857,7 @@
         <v>0.175</v>
       </c>
       <c r="Z252">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA252">
         <v>80</v>
@@ -18928,7 +18928,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z253">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA253">
         <v>80</v>
@@ -18999,7 +18999,7 @@
         <v>0.112</v>
       </c>
       <c r="Z254">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA254">
         <v>80</v>
@@ -19070,7 +19070,7 @@
         <v>0.06510000000000001</v>
       </c>
       <c r="Z255">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA255">
         <v>80</v>
@@ -19141,7 +19141,7 @@
         <v>0.098</v>
       </c>
       <c r="Z256">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA256">
         <v>80</v>
@@ -19212,7 +19212,7 @@
         <v>0.06370000000000001</v>
       </c>
       <c r="Z257">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA257">
         <v>80</v>
@@ -19286,7 +19286,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z258">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA258">
         <v>80</v>
@@ -19360,7 +19360,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z259">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA259">
         <v>80</v>
@@ -19434,7 +19434,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z260">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA260">
         <v>80</v>
@@ -19508,7 +19508,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z261">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA261">
         <v>80</v>
@@ -19582,7 +19582,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z262">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA262">
         <v>80</v>
@@ -19656,7 +19656,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z263">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA263">
         <v>80</v>
@@ -19730,7 +19730,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z264">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA264">
         <v>80</v>
@@ -19804,7 +19804,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z265">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA265">
         <v>80</v>
@@ -19875,7 +19875,7 @@
         <v>0.175</v>
       </c>
       <c r="Z266">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA266">
         <v>80</v>
@@ -19946,7 +19946,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z267">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA267">
         <v>80</v>
@@ -20017,7 +20017,7 @@
         <v>0.175</v>
       </c>
       <c r="Z268">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA268">
         <v>80</v>
@@ -20088,7 +20088,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z269">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA269">
         <v>80</v>
@@ -20159,7 +20159,7 @@
         <v>0.112</v>
       </c>
       <c r="Z270">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA270">
         <v>80</v>
@@ -20230,7 +20230,7 @@
         <v>0.06510000000000001</v>
       </c>
       <c r="Z271">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA271">
         <v>80</v>
@@ -20301,7 +20301,7 @@
         <v>0.098</v>
       </c>
       <c r="Z272">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA272">
         <v>80</v>
@@ -20372,7 +20372,7 @@
         <v>0.06370000000000001</v>
       </c>
       <c r="Z273">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA273">
         <v>80</v>
@@ -20446,7 +20446,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z274">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA274">
         <v>80</v>
@@ -20520,7 +20520,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z275">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA275">
         <v>80</v>
@@ -20594,7 +20594,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z276">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA276">
         <v>80</v>
@@ -20668,7 +20668,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z277">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA277">
         <v>80</v>
@@ -20742,7 +20742,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z278">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA278">
         <v>80</v>
@@ -20816,7 +20816,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z279">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA279">
         <v>80</v>
@@ -20890,7 +20890,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z280">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA280">
         <v>80</v>
@@ -20964,7 +20964,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z281">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA281">
         <v>80</v>
@@ -21035,7 +21035,7 @@
         <v>0.175</v>
       </c>
       <c r="Z282">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA282">
         <v>80</v>
@@ -21106,7 +21106,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z283">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA283">
         <v>80</v>
@@ -21177,7 +21177,7 @@
         <v>0.175</v>
       </c>
       <c r="Z284">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA284">
         <v>80</v>
@@ -21248,7 +21248,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z285">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA285">
         <v>80</v>
@@ -21319,7 +21319,7 @@
         <v>0.112</v>
       </c>
       <c r="Z286">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA286">
         <v>80</v>
@@ -21390,7 +21390,7 @@
         <v>0.06510000000000001</v>
       </c>
       <c r="Z287">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA287">
         <v>80</v>
@@ -21461,7 +21461,7 @@
         <v>0.098</v>
       </c>
       <c r="Z288">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA288">
         <v>80</v>
@@ -21532,7 +21532,7 @@
         <v>0.06370000000000001</v>
       </c>
       <c r="Z289">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA289">
         <v>80</v>
@@ -21606,7 +21606,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z290">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA290">
         <v>80</v>
@@ -21680,7 +21680,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z291">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA291">
         <v>80</v>
@@ -21754,7 +21754,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z292">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA292">
         <v>80</v>
@@ -21828,7 +21828,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z293">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA293">
         <v>80</v>
@@ -21902,7 +21902,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z294">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA294">
         <v>80</v>
@@ -21976,7 +21976,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z295">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA295">
         <v>80</v>
@@ -22050,7 +22050,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z296">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA296">
         <v>80</v>
@@ -22124,7 +22124,7 @@
         <v>0.004200000000000004</v>
       </c>
       <c r="Z297">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA297">
         <v>80</v>
@@ -22195,7 +22195,7 @@
         <v>0.175</v>
       </c>
       <c r="Z298">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA298">
         <v>100</v>
@@ -22266,7 +22266,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z299">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA299">
         <v>100</v>
@@ -22337,7 +22337,7 @@
         <v>0.175</v>
       </c>
       <c r="Z300">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA300">
         <v>100</v>
@@ -22408,7 +22408,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z301">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA301">
         <v>100</v>
@@ -22479,7 +22479,7 @@
         <v>0.11375</v>
       </c>
       <c r="Z302">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA302">
         <v>100</v>
@@ -22550,7 +22550,7 @@
         <v>0.04550000000000001</v>
       </c>
       <c r="Z303">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA303">
         <v>100</v>
@@ -22621,7 +22621,7 @@
         <v>0.10325</v>
       </c>
       <c r="Z304">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA304">
         <v>100</v>
@@ -22692,7 +22692,7 @@
         <v>0.04130000000000001</v>
       </c>
       <c r="Z305">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA305">
         <v>100</v>
@@ -22766,7 +22766,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z306">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA306">
         <v>100</v>
@@ -22840,7 +22840,7 @@
         <v>0.002100000000000002</v>
       </c>
       <c r="Z307">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA307">
         <v>100</v>
@@ -22914,7 +22914,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z308">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA308">
         <v>100</v>
@@ -22988,7 +22988,7 @@
         <v>0.002100000000000002</v>
       </c>
       <c r="Z309">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA309">
         <v>100</v>
@@ -23062,7 +23062,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z310">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA310">
         <v>100</v>
@@ -23136,7 +23136,7 @@
         <v>0.002100000000000002</v>
       </c>
       <c r="Z311">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA311">
         <v>100</v>
@@ -23210,7 +23210,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z312">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA312">
         <v>100</v>
@@ -23284,7 +23284,7 @@
         <v>0.002100000000000002</v>
       </c>
       <c r="Z313">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA313">
         <v>100</v>
@@ -23355,7 +23355,7 @@
         <v>0.175</v>
       </c>
       <c r="Z314">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA314">
         <v>100</v>
@@ -23426,7 +23426,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z315">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA315">
         <v>100</v>
@@ -23497,7 +23497,7 @@
         <v>0.175</v>
       </c>
       <c r="Z316">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA316">
         <v>100</v>
@@ -23568,7 +23568,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z317">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA317">
         <v>100</v>
@@ -23639,7 +23639,7 @@
         <v>0.11375</v>
       </c>
       <c r="Z318">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA318">
         <v>100</v>
@@ -23710,7 +23710,7 @@
         <v>0.04550000000000001</v>
       </c>
       <c r="Z319">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA319">
         <v>100</v>
@@ -23781,7 +23781,7 @@
         <v>0.10325</v>
       </c>
       <c r="Z320">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA320">
         <v>100</v>
@@ -23852,7 +23852,7 @@
         <v>0.04130000000000001</v>
       </c>
       <c r="Z321">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA321">
         <v>100</v>
@@ -23926,7 +23926,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z322">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA322">
         <v>100</v>
@@ -24000,7 +24000,7 @@
         <v>0.002100000000000002</v>
       </c>
       <c r="Z323">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA323">
         <v>100</v>
@@ -24074,7 +24074,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z324">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA324">
         <v>100</v>
@@ -24148,7 +24148,7 @@
         <v>0.002100000000000002</v>
       </c>
       <c r="Z325">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA325">
         <v>100</v>
@@ -24222,7 +24222,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z326">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA326">
         <v>100</v>
@@ -24296,7 +24296,7 @@
         <v>0.002100000000000002</v>
       </c>
       <c r="Z327">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA327">
         <v>100</v>
@@ -24370,7 +24370,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z328">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA328">
         <v>100</v>
@@ -24444,7 +24444,7 @@
         <v>0.002100000000000002</v>
       </c>
       <c r="Z329">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA329">
         <v>100</v>
@@ -24515,7 +24515,7 @@
         <v>0.175</v>
       </c>
       <c r="Z330">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA330">
         <v>90</v>
@@ -24586,7 +24586,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z331">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA331">
         <v>90</v>
@@ -24657,7 +24657,7 @@
         <v>0.175</v>
       </c>
       <c r="Z332">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA332">
         <v>90</v>
@@ -24728,7 +24728,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Z333">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA333">
         <v>90</v>
@@ -24799,7 +24799,7 @@
         <v>0.11375</v>
       </c>
       <c r="Z334">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA334">
         <v>90</v>
@@ -24870,7 +24870,7 @@
         <v>0.04550000000000001</v>
       </c>
       <c r="Z335">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA335">
         <v>90</v>
@@ -24941,7 +24941,7 @@
         <v>0.10325</v>
       </c>
       <c r="Z336">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA336">
         <v>90</v>
@@ -25012,7 +25012,7 @@
         <v>0.04130000000000001</v>
       </c>
       <c r="Z337">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA337">
         <v>90</v>
@@ -25086,7 +25086,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z338">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA338">
         <v>90</v>
@@ -25160,7 +25160,7 @@
         <v>0.002100000000000002</v>
       </c>
       <c r="Z339">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA339">
         <v>90</v>
@@ -25234,7 +25234,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z340">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA340">
         <v>90</v>
@@ -25308,7 +25308,7 @@
         <v>0.002100000000000002</v>
       </c>
       <c r="Z341">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA341">
         <v>90</v>
@@ -25382,7 +25382,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z342">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA342">
         <v>90</v>
@@ -25456,7 +25456,7 @@
         <v>0.002100000000000002</v>
       </c>
       <c r="Z343">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA343">
         <v>90</v>
@@ -25530,7 +25530,7 @@
         <v>0.005250000000000005</v>
       </c>
       <c r="Z344">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA344">
         <v>90</v>
@@ -25604,7 +25604,7 @@
         <v>0.002100000000000002</v>
       </c>
       <c r="Z345">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA345">
         <v>90</v>
@@ -25675,7 +25675,7 @@
         <v>0.15</v>
       </c>
       <c r="Z346">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA346">
         <v>100</v>
@@ -25746,7 +25746,7 @@
         <v>0.15</v>
       </c>
       <c r="Z347">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA347">
         <v>100</v>
@@ -25817,7 +25817,7 @@
         <v>0.09899999999999999</v>
       </c>
       <c r="Z348">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA348">
         <v>100</v>
@@ -25888,7 +25888,7 @@
         <v>0.0975</v>
       </c>
       <c r="Z349">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA349">
         <v>100</v>
@@ -25959,7 +25959,7 @@
         <v>0.02999999999999999</v>
       </c>
       <c r="Z350">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA350">
         <v>100</v>
@@ -26030,7 +26030,7 @@
         <v>0.02999999999999999</v>
       </c>
       <c r="Z351">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA351">
         <v>100</v>
@@ -26101,7 +26101,7 @@
         <v>0.01199999999999999</v>
       </c>
       <c r="Z352">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA352">
         <v>100</v>
@@ -26172,7 +26172,7 @@
         <v>0.01199999999999999</v>
       </c>
       <c r="Z353">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA353">
         <v>100</v>
@@ -26243,7 +26243,7 @@
         <v>0.01199999999999999</v>
       </c>
       <c r="Z354">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA354">
         <v>100</v>
@@ -26314,7 +26314,7 @@
         <v>0.01199999999999999</v>
       </c>
       <c r="Z355">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA355">
         <v>100</v>
@@ -26385,7 +26385,7 @@
         <v>0.01199999999999999</v>
       </c>
       <c r="Z356">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA356">
         <v>100</v>
@@ -26456,7 +26456,7 @@
         <v>0.01199999999999999</v>
       </c>
       <c r="Z357">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AA357">
         <v>100</v>

</xml_diff>